<commit_message>
update the spreadsheet, add --highlander flag to load_content
</commit_message>
<xml_diff>
--- a/fantastic_futures_inventory.xlsx
+++ b/fantastic_futures_inventory.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1072" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="313">
   <si>
     <t>Physical Format</t>
   </si>
@@ -443,18 +443,21 @@
     <t>1991 Future of the American Church Conference: Roman Catholic Fundementalists: Expanding the Matrix of interpretation</t>
   </si>
   <si>
+    <t>https://media.dlib.indiana.edu/media_objects/s1785305j</t>
+  </si>
+  <si>
+    <t>very mild background hum; otherwise good audio</t>
+  </si>
+  <si>
+    <t>Rebroadcasting of a talk by Mary Jo Weaver on the subject of catholic and protestant fundamentalism.</t>
+  </si>
+  <si>
+    <t>[United States, Indiana, Bloomington, 1975]</t>
+  </si>
+  <si>
     <t>https://media.dlib.indiana.edu/media_objects/v118s2022</t>
   </si>
   <si>
-    <t>very mild background hum; otherwise good audio</t>
-  </si>
-  <si>
-    <t>Rebroadcasting of a talk by Mary Jo Weaver on the subject of catholic and protestant fundamentalism.</t>
-  </si>
-  <si>
-    <t>[United States, Indiana, Bloomington, 1975]</t>
-  </si>
-  <si>
     <t>significant background hiss</t>
   </si>
   <si>
@@ -803,6 +806,12 @@
     <t>MDPI</t>
   </si>
   <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>40000003840917</t>
+  </si>
+  <si>
     <t>yes</t>
   </si>
   <si>
@@ -821,18 +830,33 @@
     <t>Yes</t>
   </si>
   <si>
+    <t>40000001090820</t>
+  </si>
+  <si>
     <t>45000000166352</t>
   </si>
   <si>
+    <t>45000000394467</t>
+  </si>
+  <si>
     <t>40000002486514</t>
   </si>
   <si>
+    <t>40000002867481</t>
+  </si>
+  <si>
     <t>45000000360708</t>
   </si>
   <si>
     <t>45000000360740</t>
   </si>
   <si>
+    <t>[United States, Indiana, Bloomington, Joe Heaney interview, 1980] (Tape 1 Part 1)</t>
+  </si>
+  <si>
+    <t>40000001107723</t>
+  </si>
+  <si>
     <t>40000003797083</t>
   </si>
   <si>
@@ -843,6 +867,9 @@
   </si>
   <si>
     <t>40000003525823</t>
+  </si>
+  <si>
+    <t>40000003465350</t>
   </si>
   <si>
     <t>45000000023223</t>
@@ -875,6 +902,9 @@
     <t>40000003617513</t>
   </si>
   <si>
+    <t>40000003594837</t>
+  </si>
+  <si>
     <t>40000001407792,40000001407800</t>
   </si>
   <si>
@@ -905,6 +935,9 @@
     <t>40000003421437</t>
   </si>
   <si>
+    <t>40000003805407</t>
+  </si>
+  <si>
     <t>45000000242492</t>
   </si>
   <si>
@@ -936,6 +969,18 @@
   </si>
   <si>
     <t>40000000184285</t>
+  </si>
+  <si>
+    <t>40000002521559</t>
+  </si>
+  <si>
+    <t>40000002521674</t>
+  </si>
+  <si>
+    <t>muskrat:/srv/nfs_avalon/welles/media/221.high.mp4</t>
+  </si>
+  <si>
+    <t>muskrat:/srv/nfs_avalon/welles/media/190.high.mp4</t>
   </si>
   <si>
     <t>40000003855584</t>
@@ -969,7 +1014,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1048,6 +1093,11 @@
       <color theme="1"/>
       <name val="Liberation Serif"/>
     </font>
+    <font>
+      <sz val="8.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1081,7 +1131,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1147,7 +1197,7 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="46" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="14" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0"/>
@@ -1156,6 +1206,9 @@
       <alignment horizontal="right" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="15" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="16" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -2286,7 +2339,7 @@
       <c r="D25" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="12" t="s">
         <v>128</v>
       </c>
       <c r="F25" s="6" t="s">
@@ -2323,7 +2376,7 @@
         <v>131</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>23</v>
@@ -2339,15 +2392,15 @@
         <v>104</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>20</v>
@@ -2356,10 +2409,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>31</v>
@@ -2377,7 +2430,7 @@
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>20</v>
@@ -2386,10 +2439,10 @@
         <v>28</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>63</v>
@@ -2405,12 +2458,12 @@
         <v>104</v>
       </c>
       <c r="J28" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>20</v>
@@ -2419,10 +2472,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>31</v>
@@ -2438,12 +2491,12 @@
         <v>104</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>27</v>
@@ -2452,10 +2505,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>31</v>
@@ -2471,12 +2524,12 @@
         <v>104</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>27</v>
@@ -2485,10 +2538,10 @@
         <v>28</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>31</v>
@@ -2506,7 +2559,7 @@
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>27</v>
@@ -2515,10 +2568,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>31</v>
@@ -2536,7 +2589,7 @@
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>27</v>
@@ -2545,10 +2598,10 @@
         <v>28</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>31</v>
@@ -2566,7 +2619,7 @@
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>20</v>
@@ -2575,10 +2628,10 @@
         <v>28</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>31</v>
@@ -2596,7 +2649,7 @@
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>27</v>
@@ -2605,10 +2658,10 @@
         <v>28</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>31</v>
@@ -2624,12 +2677,12 @@
         <v>32</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>60</v>
@@ -2638,10 +2691,10 @@
         <v>28</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>103</v>
@@ -2659,7 +2712,7 @@
     </row>
     <row r="37">
       <c r="A37" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>20</v>
@@ -2668,13 +2721,13 @@
         <v>28</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G37" s="9">
         <v>0.04346064814814815</v>
@@ -2688,12 +2741,12 @@
       </c>
       <c r="J37" s="18"/>
       <c r="K37" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>39</v>
@@ -2702,13 +2755,13 @@
         <v>28</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G38" s="9">
         <v>0.019050925925925926</v>
@@ -2723,7 +2776,7 @@
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>20</v>
@@ -2732,10 +2785,10 @@
         <v>28</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>63</v>
@@ -2751,12 +2804,12 @@
         <v>32</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>27</v>
@@ -2765,13 +2818,13 @@
         <v>28</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G40" s="9">
         <v>0.01892361111111111</v>
@@ -2784,12 +2837,12 @@
         <v>32</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>39</v>
@@ -2798,13 +2851,13 @@
         <v>28</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G41" s="9">
         <v>0.0437962962962963</v>
@@ -2819,7 +2872,7 @@
     </row>
     <row r="42">
       <c r="A42" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>20</v>
@@ -2828,13 +2881,13 @@
         <v>28</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G42" s="9">
         <v>0.021921296296296296</v>
@@ -2849,7 +2902,7 @@
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>20</v>
@@ -2858,13 +2911,13 @@
         <v>28</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G43" s="9">
         <v>0.047858796296296295</v>
@@ -2878,12 +2931,12 @@
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="6" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>80</v>
@@ -2892,13 +2945,13 @@
         <v>28</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G44" s="9">
         <v>0.017719907407407406</v>
@@ -2911,12 +2964,12 @@
         <v>104</v>
       </c>
       <c r="J44" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>27</v>
@@ -2925,13 +2978,13 @@
         <v>28</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G45" s="9">
         <v>0.015983796296296298</v>
@@ -2944,15 +2997,15 @@
         <v>104</v>
       </c>
       <c r="J45" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>20</v>
@@ -2961,10 +3014,10 @@
         <v>13</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>63</v>
@@ -2980,15 +3033,15 @@
         <v>32</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>20</v>
@@ -2997,10 +3050,10 @@
         <v>13</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>103</v>
@@ -3016,12 +3069,12 @@
         <v>32</v>
       </c>
       <c r="J47" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>39</v>
@@ -3030,13 +3083,13 @@
         <v>13</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G48" s="9">
         <v>0.007615740740740741</v>
@@ -3049,15 +3102,15 @@
         <v>32</v>
       </c>
       <c r="J48" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>20</v>
@@ -3066,10 +3119,10 @@
         <v>13</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>16</v>
@@ -3085,15 +3138,15 @@
         <v>32</v>
       </c>
       <c r="J49" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>20</v>
@@ -3102,10 +3155,10 @@
         <v>13</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>16</v>
@@ -3121,12 +3174,12 @@
         <v>32</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>20</v>
@@ -3135,13 +3188,13 @@
         <v>13</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G51" s="9">
         <v>0.0038657407407407408</v>
@@ -3158,7 +3211,7 @@
     </row>
     <row r="52">
       <c r="A52" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>20</v>
@@ -3167,10 +3220,10 @@
         <v>13</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>16</v>
@@ -3186,15 +3239,15 @@
         <v>64</v>
       </c>
       <c r="J52" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>20</v>
@@ -3203,10 +3256,10 @@
         <v>13</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>23</v>
@@ -3222,13 +3275,13 @@
         <v>64</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K53" s="6"/>
     </row>
     <row r="54">
       <c r="A54" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>27</v>
@@ -3237,10 +3290,10 @@
         <v>13</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>16</v>
@@ -3256,15 +3309,15 @@
         <v>64</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>80</v>
@@ -3273,10 +3326,10 @@
         <v>13</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>23</v>
@@ -3292,15 +3345,15 @@
         <v>104</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>20</v>
@@ -3309,10 +3362,10 @@
         <v>28</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>31</v>
@@ -3328,12 +3381,12 @@
         <v>104</v>
       </c>
       <c r="J56" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>27</v>
@@ -3342,10 +3395,10 @@
         <v>28</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>31</v>
@@ -3363,7 +3416,7 @@
     </row>
     <row r="58">
       <c r="A58" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>39</v>
@@ -3372,10 +3425,10 @@
         <v>28</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>63</v>
@@ -3391,12 +3444,12 @@
         <v>104</v>
       </c>
       <c r="J58" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>20</v>
@@ -3405,10 +3458,10 @@
         <v>28</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>63</v>
@@ -3424,15 +3477,15 @@
         <v>104</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>60</v>
@@ -3441,10 +3494,10 @@
         <v>28</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>63</v>
@@ -3463,7 +3516,7 @@
     <row r="61">
       <c r="D61" s="21"/>
       <c r="F61" s="6" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G61" s="22">
         <f t="shared" ref="G61:H61" si="2">sum(G2:G60)</f>
@@ -3477,7 +3530,7 @@
     <row r="62">
       <c r="D62" s="21"/>
       <c r="F62" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G62" s="23">
         <f>IFERROR(__xludf.DUMMYFUNCTION("index(split(G61,"":""),1)*60+index(split(G61,"":""),2)"),2051.0)</f>
@@ -3491,7 +3544,7 @@
     <row r="63">
       <c r="D63" s="21"/>
       <c r="F63" s="6" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="G63" s="23">
         <f t="shared" ref="G63:H63" si="3">G62*2.3</f>
@@ -3504,7 +3557,7 @@
     </row>
     <row r="64">
       <c r="A64" s="6" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D64" s="21"/>
     </row>
@@ -6505,7 +6558,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="6" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="2">
@@ -6590,7 +6643,7 @@
         <v>8</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
@@ -6599,9 +6652,11 @@
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="M1" s="4"/>
+        <v>248</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>249</v>
+      </c>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
@@ -6654,7 +6709,9 @@
       <c r="K2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="24"/>
+      <c r="L2" s="24" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
@@ -6682,7 +6739,7 @@
         <v>17</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J3" s="6" t="s">
         <v>24</v>
@@ -6691,7 +6748,7 @@
         <v>25</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4">
@@ -6727,7 +6784,7 @@
         <v>34</v>
       </c>
       <c r="L4" s="26" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5">
@@ -6763,7 +6820,7 @@
         <v>38</v>
       </c>
       <c r="L5" s="26" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6">
@@ -6799,7 +6856,7 @@
         <v>44</v>
       </c>
       <c r="L6" s="27" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7">
@@ -6828,7 +6885,7 @@
         <v>17</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>48</v>
@@ -6836,7 +6893,9 @@
       <c r="K7" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="L7" s="24"/>
+      <c r="L7" s="24" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
@@ -6871,7 +6930,7 @@
         <v>53</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>254</v>
+        <v>258</v>
       </c>
     </row>
     <row r="9">
@@ -6906,7 +6965,9 @@
       <c r="K9" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="L9" s="24"/>
+      <c r="L9" s="24" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
@@ -6933,7 +6994,9 @@
       <c r="H10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J10" s="6" t="s">
         <v>65</v>
       </c>
@@ -6941,7 +7004,7 @@
         <v>66</v>
       </c>
       <c r="L10" s="26" t="s">
-        <v>255</v>
+        <v>260</v>
       </c>
     </row>
     <row r="11">
@@ -6976,7 +7039,9 @@
       <c r="K11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="L11" s="24"/>
+      <c r="L11" s="24" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
@@ -7003,7 +7068,9 @@
       <c r="H12" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="6"/>
+      <c r="I12" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J12" s="6" t="s">
         <v>74</v>
       </c>
@@ -7011,7 +7078,7 @@
         <v>75</v>
       </c>
       <c r="L12" s="26" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
     </row>
     <row r="13">
@@ -7039,7 +7106,9 @@
       <c r="H13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I13" s="6"/>
+      <c r="I13" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J13" s="6" t="s">
         <v>78</v>
       </c>
@@ -7047,7 +7116,7 @@
         <v>79</v>
       </c>
       <c r="L13" s="26" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
     </row>
     <row r="14">
@@ -7061,7 +7130,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>81</v>
+        <v>264</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>82</v>
@@ -7070,13 +7139,13 @@
         <v>23</v>
       </c>
       <c r="G14" s="9">
-        <v>0.022962962962962963</v>
+        <v>0.02295138888888889</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>17</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J14" s="6" t="s">
         <v>83</v>
@@ -7084,7 +7153,10 @@
       <c r="K14" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="24"/>
+      <c r="L14" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="M14" s="28"/>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
@@ -7111,7 +7183,9 @@
       <c r="H15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I15" s="6"/>
+      <c r="I15" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J15" s="6" t="s">
         <v>87</v>
       </c>
@@ -7119,7 +7193,7 @@
         <v>88</v>
       </c>
       <c r="L15" s="26" t="s">
-        <v>258</v>
+        <v>266</v>
       </c>
     </row>
     <row r="16">
@@ -7155,7 +7229,7 @@
         <v>91</v>
       </c>
       <c r="L16" s="26" t="s">
-        <v>259</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17">
@@ -7189,7 +7263,7 @@
         <v>95</v>
       </c>
       <c r="L17" s="26" t="s">
-        <v>260</v>
+        <v>268</v>
       </c>
     </row>
     <row r="18">
@@ -7225,7 +7299,7 @@
         <v>100</v>
       </c>
       <c r="L18" s="26" t="s">
-        <v>261</v>
+        <v>269</v>
       </c>
     </row>
     <row r="19">
@@ -7260,7 +7334,9 @@
       <c r="K19" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="L19" s="24"/>
+      <c r="L19" s="24" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="6" t="s">
@@ -7295,7 +7371,7 @@
         <v>110</v>
       </c>
       <c r="L20" s="26" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
     </row>
     <row r="21">
@@ -7323,7 +7399,9 @@
       <c r="H21" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I21" s="6"/>
+      <c r="I21" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J21" s="6" t="s">
         <v>113</v>
       </c>
@@ -7331,7 +7409,7 @@
         <v>114</v>
       </c>
       <c r="L21" s="26" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="22">
@@ -7348,7 +7426,7 @@
         <v>115</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>63</v>
@@ -7359,7 +7437,9 @@
       <c r="H22" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="I22" s="6"/>
+      <c r="I22" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J22" s="6" t="s">
         <v>117</v>
       </c>
@@ -7367,7 +7447,7 @@
         <v>118</v>
       </c>
       <c r="L22" s="26" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="23">
@@ -7395,7 +7475,9 @@
       <c r="H23" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J23" s="6" t="s">
         <v>121</v>
       </c>
@@ -7403,7 +7485,7 @@
         <v>122</v>
       </c>
       <c r="L23" s="26" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="24">
@@ -7431,7 +7513,9 @@
       <c r="H24" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="6"/>
+      <c r="I24" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J24" s="6" t="s">
         <v>125</v>
       </c>
@@ -7439,7 +7523,7 @@
         <v>126</v>
       </c>
       <c r="L24" s="26" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25">
@@ -7467,14 +7551,18 @@
       <c r="H25" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I25" s="6"/>
+      <c r="I25" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J25" s="6" t="s">
         <v>129</v>
       </c>
       <c r="K25" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="L25" s="24"/>
+      <c r="L25" s="24" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="6" t="s">
@@ -7490,7 +7578,7 @@
         <v>131</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>23</v>
@@ -7502,21 +7590,21 @@
         <v>104</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L26" s="27" t="s">
-        <v>268</v>
+        <v>278</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>20</v>
@@ -7525,10 +7613,10 @@
         <v>28</v>
       </c>
       <c r="D27" s="14" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>31</v>
@@ -7540,12 +7628,12 @@
         <v>104</v>
       </c>
       <c r="L27" s="26" t="s">
-        <v>269</v>
+        <v>279</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>20</v>
@@ -7554,10 +7642,10 @@
         <v>28</v>
       </c>
       <c r="D28" s="14" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>63</v>
@@ -7568,17 +7656,19 @@
       <c r="H28" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I28" s="6"/>
+      <c r="I28" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J28" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="L28" s="26" t="s">
-        <v>270</v>
+        <v>280</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>20</v>
@@ -7587,10 +7677,10 @@
         <v>28</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>31</v>
@@ -7602,15 +7692,15 @@
         <v>104</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="L29" s="26" t="s">
-        <v>271</v>
+        <v>281</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>27</v>
@@ -7619,10 +7709,10 @@
         <v>28</v>
       </c>
       <c r="D30" s="17" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>31</v>
@@ -7634,15 +7724,15 @@
         <v>104</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="L30" s="26" t="s">
-        <v>272</v>
+        <v>282</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>27</v>
@@ -7651,10 +7741,10 @@
         <v>28</v>
       </c>
       <c r="D31" s="17" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="E31" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>31</v>
@@ -7666,12 +7756,12 @@
         <v>104</v>
       </c>
       <c r="L31" s="26" t="s">
-        <v>273</v>
+        <v>283</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>27</v>
@@ -7680,10 +7770,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>31</v>
@@ -7695,12 +7785,12 @@
         <v>104</v>
       </c>
       <c r="L32" s="26" t="s">
-        <v>274</v>
+        <v>284</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>27</v>
@@ -7709,10 +7799,10 @@
         <v>28</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E33" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>31</v>
@@ -7724,12 +7814,12 @@
         <v>104</v>
       </c>
       <c r="L33" s="26" t="s">
-        <v>275</v>
+        <v>285</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>20</v>
@@ -7738,10 +7828,10 @@
         <v>28</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E34" s="8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>31</v>
@@ -7753,12 +7843,12 @@
         <v>104</v>
       </c>
       <c r="L34" s="26" t="s">
-        <v>276</v>
+        <v>286</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>27</v>
@@ -7767,10 +7857,10 @@
         <v>28</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>31</v>
@@ -7782,15 +7872,15 @@
         <v>32</v>
       </c>
       <c r="K35" s="6" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="L35" s="26" t="s">
-        <v>277</v>
+        <v>287</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>60</v>
@@ -7799,10 +7889,10 @@
         <v>28</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E36" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>103</v>
@@ -7813,11 +7903,13 @@
       <c r="H36" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L36" s="24"/>
+      <c r="L36" s="24" t="s">
+        <v>288</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>20</v>
@@ -7826,13 +7918,13 @@
         <v>28</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E37" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G37" s="9">
         <v>0.04346064814814815</v>
@@ -7843,15 +7935,15 @@
       <c r="I37" s="18"/>
       <c r="J37" s="18"/>
       <c r="K37" s="6" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L37" s="26" t="s">
-        <v>278</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>39</v>
@@ -7860,13 +7952,13 @@
         <v>28</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E38" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G38" s="9">
         <v>0.019050925925925926</v>
@@ -7875,12 +7967,12 @@
         <v>32</v>
       </c>
       <c r="L38" s="26" t="s">
-        <v>279</v>
+        <v>290</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>20</v>
@@ -7889,10 +7981,10 @@
         <v>28</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E39" s="8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>63</v>
@@ -7903,16 +7995,19 @@
       <c r="H39" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="I39" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="K39" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="L39" s="26" t="s">
-        <v>280</v>
+        <v>291</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>27</v>
@@ -7921,13 +8016,13 @@
         <v>28</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G40" s="9">
         <v>0.01892361111111111</v>
@@ -7936,15 +8031,15 @@
         <v>32</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="L40" s="26" t="s">
-        <v>281</v>
+        <v>292</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>39</v>
@@ -7953,13 +8048,13 @@
         <v>28</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="E41" s="8" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G41" s="9">
         <v>0.0437962962962963</v>
@@ -7968,12 +8063,12 @@
         <v>32</v>
       </c>
       <c r="L41" s="26" t="s">
-        <v>282</v>
+        <v>293</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>20</v>
@@ -7982,13 +8077,13 @@
         <v>28</v>
       </c>
       <c r="D42" s="17" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E42" s="8" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G42" s="9">
         <v>0.021921296296296296</v>
@@ -7997,12 +8092,12 @@
         <v>32</v>
       </c>
       <c r="L42" s="26" t="s">
-        <v>283</v>
+        <v>294</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>12</v>
@@ -8011,13 +8106,13 @@
         <v>28</v>
       </c>
       <c r="D43" s="7" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="G43" s="9">
         <v>0.047858796296296295</v>
@@ -8026,19 +8121,19 @@
         <v>64</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="J43" s="6"/>
       <c r="K43" s="6" t="s">
-        <v>284</v>
+        <v>295</v>
       </c>
       <c r="L43" s="26" t="s">
-        <v>285</v>
+        <v>296</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>80</v>
@@ -8047,13 +8142,13 @@
         <v>28</v>
       </c>
       <c r="D44" s="14" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G44" s="9">
         <v>0.017719907407407406</v>
@@ -8063,15 +8158,15 @@
       </c>
       <c r="I44" s="6"/>
       <c r="J44" s="6" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="L44" s="26" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="6" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>27</v>
@@ -8080,13 +8175,13 @@
         <v>28</v>
       </c>
       <c r="D45" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="G45" s="9">
         <v>0.015983796296296298</v>
@@ -8096,18 +8191,18 @@
       </c>
       <c r="I45" s="6"/>
       <c r="J45" s="6" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="L45" s="26" t="s">
-        <v>287</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>20</v>
@@ -8116,10 +8211,10 @@
         <v>13</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>63</v>
@@ -8130,20 +8225,22 @@
       <c r="H46" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I46" s="6"/>
+      <c r="I46" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J46" s="6" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="K46" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="L46" s="26" t="s">
-        <v>288</v>
+        <v>299</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>20</v>
@@ -8152,10 +8249,10 @@
         <v>13</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E47" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>103</v>
@@ -8168,13 +8265,15 @@
       </c>
       <c r="I47" s="6"/>
       <c r="J47" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="L47" s="24"/>
+        <v>197</v>
+      </c>
+      <c r="L47" s="24" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>39</v>
@@ -8183,13 +8282,13 @@
         <v>13</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E48" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G48" s="9">
         <v>0.007615740740740741</v>
@@ -8199,16 +8298,18 @@
       </c>
       <c r="I48" s="6"/>
       <c r="J48" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="K48" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="L48" s="24"/>
+        <v>202</v>
+      </c>
+      <c r="L48" s="24" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>20</v>
@@ -8217,10 +8318,10 @@
         <v>13</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>16</v>
@@ -8233,16 +8334,18 @@
       </c>
       <c r="I49" s="6"/>
       <c r="J49" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="K49" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="L49" s="24"/>
+        <v>206</v>
+      </c>
+      <c r="L49" s="28" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>20</v>
@@ -8251,10 +8354,10 @@
         <v>13</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>16</v>
@@ -8267,13 +8370,15 @@
       </c>
       <c r="I50" s="6"/>
       <c r="J50" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="L50" s="24"/>
+        <v>209</v>
+      </c>
+      <c r="L50" s="28" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="6" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>20</v>
@@ -8282,13 +8387,13 @@
         <v>13</v>
       </c>
       <c r="D51" s="17" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G51" s="9">
         <v>0.0038657407407407408</v>
@@ -8300,12 +8405,12 @@
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="26" t="s">
-        <v>289</v>
+        <v>304</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>20</v>
@@ -8314,10 +8419,10 @@
         <v>13</v>
       </c>
       <c r="D52" s="17" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="E52" s="8" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>16</v>
@@ -8330,18 +8435,18 @@
       </c>
       <c r="I52" s="6"/>
       <c r="J52" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K52" s="6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L52" s="26" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>20</v>
@@ -8350,10 +8455,10 @@
         <v>13</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E53" s="12" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>23</v>
@@ -8365,19 +8470,19 @@
         <v>64</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J53" s="6" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="K53" s="6"/>
       <c r="L53" s="26" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>27</v>
@@ -8386,10 +8491,10 @@
         <v>13</v>
       </c>
       <c r="D54" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E54" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>16</v>
@@ -8402,18 +8507,18 @@
       </c>
       <c r="I54" s="6"/>
       <c r="J54" s="6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K54" s="6" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L54" s="25" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>80</v>
@@ -8422,10 +8527,10 @@
         <v>13</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E55" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>23</v>
@@ -8437,21 +8542,21 @@
         <v>104</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="J55" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L55" s="27" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>20</v>
@@ -8460,10 +8565,10 @@
         <v>28</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E56" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F56" s="6" t="s">
         <v>31</v>
@@ -8476,15 +8581,15 @@
       </c>
       <c r="I56" s="6"/>
       <c r="J56" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="L56" s="26" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>27</v>
@@ -8493,10 +8598,10 @@
         <v>28</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>31</v>
@@ -8508,12 +8613,12 @@
         <v>104</v>
       </c>
       <c r="L57" s="26" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>39</v>
@@ -8522,10 +8627,10 @@
         <v>28</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E58" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>63</v>
@@ -8536,17 +8641,19 @@
       <c r="H58" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I58" s="6"/>
+      <c r="I58" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J58" s="6" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="L58" s="26" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>20</v>
@@ -8555,10 +8662,10 @@
         <v>28</v>
       </c>
       <c r="D59" s="17" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="E59" s="8" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>63</v>
@@ -8569,20 +8676,22 @@
       <c r="H59" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="I59" s="6"/>
+      <c r="I59" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="J59" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="K59" s="6" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L59" s="26" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="6" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>60</v>
@@ -8591,10 +8700,10 @@
         <v>28</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="E60" s="8" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>63</v>
@@ -8605,8 +8714,11 @@
       <c r="H60" s="6" t="s">
         <v>104</v>
       </c>
+      <c r="I60" s="6" t="s">
+        <v>251</v>
+      </c>
       <c r="L60" s="26" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
     </row>
     <row r="61" ht="23.25" customHeight="1">

</xml_diff>